<commit_message>
Fix errors in M54/M52TU iat scale
</commit_message>
<xml_diff>
--- a/m52tu-m54_PnP/M52TU-M54 temp sensor calibrations.xlsx
+++ b/m52tu-m54_PnP/M52TU-M54 temp sensor calibrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52tu, m54 PnP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52tu-m54_PnP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD73328A-BEFD-44CD-98F5-4ED5801A1EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1935958F-CB8A-4794-9B66-7FDE93A7DE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28530" yWindow="690" windowWidth="27975" windowHeight="15570" xr2:uid="{82CE32EB-BF3E-452E-A707-F10BC49B34FC}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="29115" windowHeight="19650" xr2:uid="{82CE32EB-BF3E-452E-A707-F10BC49B34FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,9 +163,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -203,7 +203,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -309,7 +309,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,7 +451,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E041B05A-DAB4-4FE4-A52A-6BC53413C950}">
   <dimension ref="C1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
         <v>-48</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="0"/>
+        <f>(C19*$K$3)/(5-C19)</f>
         <v>141930.6206896556</v>
       </c>
       <c r="G19" s="1">
@@ -1023,7 +1023,7 @@
         <v>2.0920000000000001</v>
       </c>
       <c r="D31" s="1">
-        <v>39.799999999999997</v>
+        <v>50.3</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="2"/>
@@ -1041,7 +1041,7 @@
         <v>3.089</v>
       </c>
       <c r="D32" s="1">
-        <v>20.3</v>
+        <v>30</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="2"/>
@@ -1123,7 +1123,7 @@
         <v>4.9269999999999996</v>
       </c>
       <c r="D37" s="1">
-        <v>-30</v>
+        <v>-39.799999999999997</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="2"/>

</xml_diff>